<commit_message>
move xoffset,yoffset into s2cfg and out of function params
</commit_message>
<xml_diff>
--- a/xls/baremetrics_metric1.xlsx
+++ b/xls/baremetrics_metric1.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="-5160" yWindow="900" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="subs" sheetId="1" r:id="rId1"/>
     <sheet name="data" sheetId="3" r:id="rId2"/>
     <sheet name="s2cfg" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" calcOnSave="0"/>
+  <calcPr calcId="125725" calcOnSave="0"/>
 </workbook>
 </file>
 
@@ -66,11 +66,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,20 +120,18 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.f32bde48526c4ea8b8fce509c66e63bb">
+    <main first="rtdsrv.8a6ebd991163445cb0e3ec69bab38b8f">
+      <tp t="s">
+        <v>0</v>
+        <stp/>
+        <stp>baremetrics.metricQuery1.count</stp>
+        <tr r="B2" s="1"/>
+      </tp>
       <tp t="s">
         <v>complete</v>
         <stp/>
         <stp>baremetrics.metricQuery1.status</stp>
         <tr r="B3" s="1"/>
-      </tp>
-    </main>
-    <main first="rtdsrv.f32bde48526c4ea8b8fce509c66e63bb">
-      <tp t="s">
-        <v>0</v>
-        <stp/>
-        <stp>baremetrics.metricQuery1.count</stp>
-        <tr r="B2" s="1"/>
       </tp>
     </main>
   </volType>
@@ -215,7 +213,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -250,7 +247,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,21 +422,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -449,7 +445,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -458,7 +454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -473,15 +469,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -498,186 +494,186 @@
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="B1" s="2" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-04-15</v>
+        <v>2017-04-19</v>
       </c>
       <c r="C1" s="2" t="str">
         <f>_xll.s2today(-6)</f>
-        <v>2017-04-16</v>
+        <v>2017-04-20</v>
       </c>
       <c r="D1" s="2" t="str">
         <f>_xll.s2today(-5)</f>
-        <v>2017-04-17</v>
+        <v>2017-04-21</v>
       </c>
       <c r="E1" s="2" t="str">
         <f>_xll.s2today(-4)</f>
-        <v>2017-04-18</v>
+        <v>2017-04-22</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>_xll.s2today(-3)</f>
-        <v>2017-04-19</v>
+        <v>2017-04-23</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>_xll.s2today(-2)</f>
-        <v>2017-04-20</v>
+        <v>2017-04-24</v>
       </c>
       <c r="H1" s="2" t="str">
         <f>_xll.s2today(-1)</f>
-        <v>2017-04-21</v>
+        <v>2017-04-25</v>
       </c>
       <c r="I1" s="2" t="str">
         <f>_xll.s2today(0)</f>
-        <v>2017-04-22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2017-04-26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="e">
+      <c r="B2">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C2" t="e">
+        <v>0</v>
+      </c>
+      <c r="C2">
         <f>_xll.s2bcache( subs!$A$1,C$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D2" t="e">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <f>_xll.s2bcache( subs!$A$1,D$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E2" t="e">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <f>_xll.s2bcache( subs!$A$1,E$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F2" t="e">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <f>_xll.s2bcache( subs!$A$1,F$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G2" t="e">
+        <v>0</v>
+      </c>
+      <c r="G2">
         <f>_xll.s2bcache( subs!$A$1,G$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H2" t="e">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <f>_xll.s2bcache( subs!$A$1,H$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I2" t="e">
+        <v>0</v>
+      </c>
+      <c r="I2">
         <f>_xll.s2bcache( subs!$A$1,I$1,$A2)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="e">
+      <c r="B3">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C3" t="e">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <f>_xll.s2bcache( subs!$A$1,C$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D3" t="e">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <f>_xll.s2bcache( subs!$A$1,D$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E3" t="e">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <f>_xll.s2bcache( subs!$A$1,E$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F3" t="e">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <f>_xll.s2bcache( subs!$A$1,F$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G3" t="e">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <f>_xll.s2bcache( subs!$A$1,G$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H3" t="e">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <f>_xll.s2bcache( subs!$A$1,H$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I3" t="e">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <f>_xll.s2bcache( subs!$A$1,I$1,$A3)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="e">
+      <c r="B4">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C4" t="e">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <f>_xll.s2bcache( subs!$A$1,C$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D4" t="e">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <f>_xll.s2bcache( subs!$A$1,D$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E4" t="e">
+        <v>0</v>
+      </c>
+      <c r="E4">
         <f>_xll.s2bcache( subs!$A$1,E$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F4" t="e">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <f>_xll.s2bcache( subs!$A$1,F$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G4" t="e">
+        <v>0</v>
+      </c>
+      <c r="G4">
         <f>_xll.s2bcache( subs!$A$1,G$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H4" t="e">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <f>_xll.s2bcache( subs!$A$1,H$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I4" t="e">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <f>_xll.s2bcache( subs!$A$1,I$1,$A4)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="e">
+      <c r="B5">
         <f>_xll.s2bcache( subs!$A$1,B$1,$A5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="C5" t="e">
+        <v>0</v>
+      </c>
+      <c r="C5">
         <f>_xll.s2bcache( subs!$A$1,C$1,$A5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D5" t="e">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <f>_xll.s2bcache( subs!$A$1,D$1,$A5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E5" t="e">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <f>_xll.s2bcache( subs!$A$1,E$1,$A5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="F5" t="e">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <f>_xll.s2bcache( subs!$A$1,F$1,$A5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="G5" t="e">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <f>_xll.s2bcache( subs!$A$1,G$1,$A5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="H5" t="e">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <f>_xll.s2bcache( subs!$A$1,H$1,$A5)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="I5" t="e">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <f>_xll.s2bcache( subs!$A$1,I$1,$A5)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -686,7 +682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -694,7 +690,7 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -706,7 +702,7 @@
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -733,14 +729,14 @@
       </c>
       <c r="I1" s="1" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-04-15</v>
+        <v>2017-04-19</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="str">
         <f>_xll.s2today( 0)</f>
-        <v>2017-04-22</v>
+        <v>2017-04-26</v>
       </c>
       <c r="L1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Fix s2bcache access to child arrays
</commit_message>
<xml_diff>
--- a/xls/baremetrics_metric1.xlsx
+++ b/xls/baremetrics_metric1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-5160" yWindow="900" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-5160" yWindow="900" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="subs" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,282 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Windows User</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Define this s2cfg row as a baremetrics query.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+"query" not "config" or "comment"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+QueryKey referenced by calls to s2sub, s2bcache and s2baremetrics.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+"qtype" in this cell signals that it's neighbour specifies which type of baremetrics query: summary, metric or plan.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This field should be summary, metric or plan. In this case it's metric.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Another key in a key value pair, signalling that the next field defines which type of metric. See Available Metrics in the baremetrics docs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+We're getting mrr. Could also be arpu, arr, ltv etc.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Signals that the next field is the start of the date range.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Get the date for a week ago, using non volatile s2today. Don't use Excel's TODAY: it causes an endless calc cycle!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Signals that the next field is the end of the date range.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Windows User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Today's date, using non volatile s2today.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>query</t>
   </si>
@@ -37,9 +311,6 @@
   </si>
   <si>
     <t>end_date</t>
-  </si>
-  <si>
-    <t>sandbox</t>
   </si>
   <si>
     <t>mrr</t>
@@ -70,13 +341,26 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,18 +404,20 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
-    <main first="rtdsrv.8a6ebd991163445cb0e3ec69bab38b8f">
-      <tp t="s">
-        <v>0</v>
-        <stp/>
-        <stp>baremetrics.metricQuery1.count</stp>
-        <tr r="B2" s="1"/>
-      </tp>
+    <main first="rtdsrv.efe361c41fe341529c2dd667a94cb75b">
       <tp t="s">
         <v>complete</v>
         <stp/>
         <stp>baremetrics.metricQuery1.status</stp>
         <tr r="B3" s="1"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.efe361c41fe341529c2dd667a94cb75b">
+      <tp t="s">
+        <v>8</v>
+        <stp/>
+        <stp>baremetrics.metricQuery1.count</stp>
+        <tr r="B2" s="1"/>
       </tp>
     </main>
   </volType>
@@ -426,8 +712,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -438,7 +724,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="str">
         <f>_xll.s2baremetrics(A1)</f>
@@ -451,7 +737,7 @@
       </c>
       <c r="B2" t="str">
         <f>_xll.s2sub(s2cfg!$A$1,$A$1,A2)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -473,8 +759,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -497,183 +783,183 @@
     <row r="1" spans="1:9">
       <c r="B1" s="2" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-04-19</v>
+        <v>2017-05-04</v>
       </c>
       <c r="C1" s="2" t="str">
         <f>_xll.s2today(-6)</f>
-        <v>2017-04-20</v>
+        <v>2017-05-05</v>
       </c>
       <c r="D1" s="2" t="str">
         <f>_xll.s2today(-5)</f>
-        <v>2017-04-21</v>
+        <v>2017-05-06</v>
       </c>
       <c r="E1" s="2" t="str">
         <f>_xll.s2today(-4)</f>
-        <v>2017-04-22</v>
+        <v>2017-05-07</v>
       </c>
       <c r="F1" s="2" t="str">
         <f>_xll.s2today(-3)</f>
-        <v>2017-04-23</v>
+        <v>2017-05-08</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>_xll.s2today(-2)</f>
-        <v>2017-04-24</v>
+        <v>2017-05-09</v>
       </c>
       <c r="H1" s="2" t="str">
         <f>_xll.s2today(-1)</f>
-        <v>2017-04-25</v>
+        <v>2017-05-10</v>
       </c>
       <c r="I1" s="2" t="str">
         <f>_xll.s2today(0)</f>
-        <v>2017-04-26</v>
+        <v>2017-05-11</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <f>_xll.s2bcache( subs!$A$1,B$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <f>_xll.s2bcache( subs!$A$1,C$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <f>_xll.s2bcache( subs!$A$1,D$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>_xll.s2bcache( subs!$A$1,E$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <f>_xll.s2bcache( subs!$A$1,F$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <f>_xll.s2bcache( subs!$A$1,G$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f>_xll.s2bcache( subs!$A$1,H$1,$A2)</f>
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <f>_xll.s2bcache( subs!$A$1,I$1,$A2)</f>
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A2, subs!$B$2)</f>
+        <v>500</v>
+      </c>
+      <c r="C2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A2, subs!$B$2)</f>
+        <v>500</v>
+      </c>
+      <c r="D2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A2, subs!$B$2)</f>
+        <v>500</v>
+      </c>
+      <c r="E2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A2, subs!$B$2)</f>
+        <v>500</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A2, subs!$B$2)</f>
+        <v>500</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A2, subs!$B$2)</f>
+        <v>500</v>
+      </c>
+      <c r="H2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A2, subs!$B$2)</f>
+        <v>20600</v>
+      </c>
+      <c r="I2" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A2, subs!$B$2)</f>
+        <v>20600</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <f>_xll.s2bcache( subs!$A$1,B$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <f>_xll.s2bcache( subs!$A$1,C$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <f>_xll.s2bcache( subs!$A$1,D$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f>_xll.s2bcache( subs!$A$1,E$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <f>_xll.s2bcache( subs!$A$1,F$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <f>_xll.s2bcache( subs!$A$1,G$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f>_xll.s2bcache( subs!$A$1,H$1,$A3)</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f>_xll.s2bcache( subs!$A$1,I$1,$A3)</f>
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="B3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A3, subs!$B$2)</f>
+        <v>2017-04-04</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A3, subs!$B$2)</f>
+        <v>2017-04-05</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A3, subs!$B$2)</f>
+        <v>2017-04-06</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A3, subs!$B$2)</f>
+        <v>2017-04-07</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A3, subs!$B$2)</f>
+        <v>2017-04-08</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A3, subs!$B$2)</f>
+        <v>2017-04-09</v>
+      </c>
+      <c r="H3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A3, subs!$B$2)</f>
+        <v>2017-04-10</v>
+      </c>
+      <c r="I3" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A3, subs!$B$2)</f>
+        <v>2017-04-11</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4">
-        <f>_xll.s2bcache( subs!$A$1,B$1,$A4)</f>
+        <v>12</v>
+      </c>
+      <c r="B4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
-      <c r="C4">
-        <f>_xll.s2bcache( subs!$A$1,C$1,$A4)</f>
+      <c r="C4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
-      <c r="D4">
-        <f>_xll.s2bcache( subs!$A$1,D$1,$A4)</f>
+      <c r="D4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
-      <c r="E4">
-        <f>_xll.s2bcache( subs!$A$1,E$1,$A4)</f>
+      <c r="E4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
-      <c r="F4">
-        <f>_xll.s2bcache( subs!$A$1,F$1,$A4)</f>
+      <c r="F4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
-      <c r="G4">
-        <f>_xll.s2bcache( subs!$A$1,G$1,$A4)</f>
+      <c r="G4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
-      <c r="H4">
-        <f>_xll.s2bcache( subs!$A$1,H$1,$A4)</f>
+      <c r="H4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
-      <c r="I4">
-        <f>_xll.s2bcache( subs!$A$1,I$1,$A4)</f>
+      <c r="I4" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A4, subs!$B$2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <f>_xll.s2bcache( subs!$A$1,B$1,$A5)</f>
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <f>_xll.s2bcache( subs!$A$1,C$1,$A5)</f>
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <f>_xll.s2bcache( subs!$A$1,D$1,$A5)</f>
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>_xll.s2bcache( subs!$A$1,E$1,$A5)</f>
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <f>_xll.s2bcache( subs!$A$1,F$1,$A5)</f>
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <f>_xll.s2bcache( subs!$A$1,G$1,$A5)</f>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f>_xll.s2bcache( subs!$A$1,H$1,$A5)</f>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f>_xll.s2bcache( subs!$A$1,I$1,$A5)</f>
-        <v>0</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,B$1,$A5, subs!$B$2)</f>
+        <v>100</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,C$1,$A5, subs!$B$2)</f>
+        <v>100</v>
+      </c>
+      <c r="D5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,D$1,$A5, subs!$B$2)</f>
+        <v>100</v>
+      </c>
+      <c r="E5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,E$1,$A5, subs!$B$2)</f>
+        <v>100</v>
+      </c>
+      <c r="F5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,F$1,$A5, subs!$B$2)</f>
+        <v>100</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,G$1,$A5, subs!$B$2)</f>
+        <v>100</v>
+      </c>
+      <c r="H5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,H$1,$A5, subs!$B$2)</f>
+        <v>100</v>
+      </c>
+      <c r="I5" t="str">
+        <f>_xll.s2bcache( subs!$A$1,I$1,$A5, subs!$B$2)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -684,10 +970,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -702,7 +988,7 @@
     <col min="11" max="11" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -710,43 +996,38 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" s="1" t="str">
         <f>_xll.s2today(-7)</f>
-        <v>2017-04-19</v>
+        <v>2017-05-04</v>
       </c>
       <c r="J1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="str">
         <f>_xll.s2today( 0)</f>
-        <v>2017-04-26</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="b">
-        <v>1</v>
+        <v>2017-05-11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>